<commit_message>
Aula13 - 26/09 - Finalizando FPA
</commit_message>
<xml_diff>
--- a/FerramentaFPAProfRJPAutomaticaLock.xlsx
+++ b/FerramentaFPAProfRJPAutomaticaLock.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\Governanca-e-Melhores-Praticas-em-TI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBEF3F00-5B88-474A-AF60-C7E2BC92472E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF5FCCD6-A93C-4182-9505-43763E18183F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pontos Nao Ajustados" sheetId="1" r:id="rId1"/>
@@ -1720,7 +1720,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N424"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -2151,9 +2151,9 @@
       <c r="A24" s="31"/>
       <c r="B24" s="32"/>
       <c r="C24" s="31"/>
-      <c r="D24" s="32"/>
+      <c r="D24" s="29"/>
       <c r="E24" s="31"/>
-      <c r="F24" s="32"/>
+      <c r="F24" s="29"/>
       <c r="G24" s="39" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -2167,9 +2167,9 @@
       <c r="A25" s="31"/>
       <c r="B25" s="32"/>
       <c r="C25" s="31"/>
-      <c r="D25" s="32"/>
+      <c r="D25" s="29"/>
       <c r="E25" s="31"/>
-      <c r="F25" s="32"/>
+      <c r="F25" s="29"/>
       <c r="G25" s="39" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -2183,9 +2183,9 @@
       <c r="A26" s="31"/>
       <c r="B26" s="32"/>
       <c r="C26" s="31"/>
-      <c r="D26" s="32"/>
+      <c r="D26" s="29"/>
       <c r="E26" s="31"/>
-      <c r="F26" s="32"/>
+      <c r="F26" s="29"/>
       <c r="G26" s="39" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -2199,9 +2199,9 @@
       <c r="A27" s="31"/>
       <c r="B27" s="32"/>
       <c r="C27" s="31"/>
-      <c r="D27" s="32"/>
+      <c r="D27" s="29"/>
       <c r="E27" s="31"/>
-      <c r="F27" s="32"/>
+      <c r="F27" s="29"/>
       <c r="G27" s="39" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -2215,9 +2215,9 @@
       <c r="A28" s="31"/>
       <c r="B28" s="32"/>
       <c r="C28" s="31"/>
-      <c r="D28" s="32"/>
+      <c r="D28" s="29"/>
       <c r="E28" s="31"/>
-      <c r="F28" s="32"/>
+      <c r="F28" s="29"/>
       <c r="G28" s="39" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -2231,9 +2231,9 @@
       <c r="A29" s="31"/>
       <c r="B29" s="32"/>
       <c r="C29" s="31"/>
-      <c r="D29" s="32"/>
+      <c r="D29" s="29"/>
       <c r="E29" s="31"/>
-      <c r="F29" s="32"/>
+      <c r="F29" s="29"/>
       <c r="G29" s="39" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -2247,9 +2247,9 @@
       <c r="A30" s="31"/>
       <c r="B30" s="32"/>
       <c r="C30" s="31"/>
-      <c r="D30" s="32"/>
+      <c r="D30" s="29"/>
       <c r="E30" s="31"/>
-      <c r="F30" s="32"/>
+      <c r="F30" s="29"/>
       <c r="G30" s="39" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -2263,9 +2263,9 @@
       <c r="A31" s="31"/>
       <c r="B31" s="32"/>
       <c r="C31" s="31"/>
-      <c r="D31" s="32"/>
+      <c r="D31" s="29"/>
       <c r="E31" s="31"/>
-      <c r="F31" s="32"/>
+      <c r="F31" s="29"/>
       <c r="G31" s="39" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -2279,9 +2279,9 @@
       <c r="A32" s="31"/>
       <c r="B32" s="32"/>
       <c r="C32" s="31"/>
-      <c r="D32" s="32"/>
+      <c r="D32" s="29"/>
       <c r="E32" s="31"/>
-      <c r="F32" s="32"/>
+      <c r="F32" s="29"/>
       <c r="G32" s="39" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -11166,8 +11166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11206,20 +11206,24 @@
       </c>
       <c r="F5">
         <f>0.65+(0.01*C20)</f>
-        <v>0.65</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="22"/>
+      <c r="C6" s="22">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="23"/>
+      <c r="C7" s="23">
+        <v>0</v>
+      </c>
       <c r="E7" t="s">
         <v>48</v>
       </c>
@@ -11232,80 +11236,104 @@
       <c r="B8" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="23"/>
+      <c r="C8" s="23">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B9" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="23"/>
+      <c r="C9" s="23">
+        <v>1</v>
+      </c>
       <c r="E9" s="12" t="s">
         <v>47</v>
       </c>
       <c r="F9" s="12">
         <f>F5*F7</f>
-        <v>35.1</v>
+        <v>49.68</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="23"/>
+      <c r="C10" s="23">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="23"/>
+      <c r="C11" s="23">
+        <v>5</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="23"/>
+      <c r="C12" s="23">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="23"/>
+      <c r="C13" s="23">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="23"/>
+      <c r="C14" s="23">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="23"/>
+      <c r="C15" s="23">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="23"/>
+      <c r="C16" s="23">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="23"/>
+      <c r="C17" s="23">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="23"/>
+      <c r="C18" s="23">
+        <v>3</v>
+      </c>
     </row>
     <row r="19" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="24"/>
+      <c r="C19" s="24">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="2:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B20" s="13" t="s">
@@ -11313,7 +11341,7 @@
       </c>
       <c r="C20" s="14">
         <f>SUM(C6:C19)</f>
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>